<commit_message>
Elektrik ve internet arayüzü tanımlandı
</commit_message>
<xml_diff>
--- a/kurum.xlsx
+++ b/kurum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\MEB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vsCode\mySplit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2838BB0D-1DF7-4CB2-949B-0851A7EAB2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BC28AD-E0B9-455D-B87F-8114D0DA66C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="83">
   <si>
     <t>İL</t>
   </si>
@@ -260,6 +260,15 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>7820458686</t>
+  </si>
+  <si>
+    <t>İlçe Milli Eğitim Müdürlüğü</t>
+  </si>
+  <si>
+    <t>MEM</t>
   </si>
 </sst>
 </file>
@@ -641,36 +650,38 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.88671875" customWidth="1"/>
-    <col min="6" max="6" width="35.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" customWidth="1"/>
-    <col min="10" max="10" width="17.5546875" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1"/>
-    <col min="12" max="12" width="27.109375" customWidth="1"/>
-    <col min="13" max="13" width="32.33203125" customWidth="1"/>
-    <col min="14" max="14" width="29.44140625" customWidth="1"/>
-    <col min="15" max="15" width="34.5546875" customWidth="1"/>
-    <col min="16" max="16" width="25.88671875" customWidth="1"/>
-    <col min="17" max="17" width="23.88671875" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="27.140625" customWidth="1"/>
+    <col min="13" max="13" width="32.28515625" customWidth="1"/>
+    <col min="14" max="14" width="29.42578125" customWidth="1"/>
+    <col min="15" max="15" width="34.5703125" customWidth="1"/>
+    <col min="16" max="16" width="25.85546875" customWidth="1"/>
+    <col min="17" max="17" width="23.85546875" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
     <col min="19" max="19" width="21" customWidth="1"/>
     <col min="20" max="20" width="29" customWidth="1"/>
-    <col min="21" max="21" width="20.109375" customWidth="1"/>
+    <col min="21" max="21" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,7 +746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -800,7 +811,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -865,7 +876,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -930,7 +941,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -995,7 +1006,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -1060,7 +1071,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1125,7 +1136,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1190,7 +1201,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1255,7 +1266,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1320,7 +1331,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1385,7 +1396,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -1450,7 +1461,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -1515,7 +1526,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1580,7 +1591,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1645,7 +1656,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1710,7 +1721,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1775,7 +1786,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1840,7 +1851,7 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1905,50 +1916,87 @@
         <v>45411.384398148148</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5" t="s">
+    <row r="20" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="3">
+        <v>127776</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="4"/>
+    </row>
+    <row r="21" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6" t="s">
+      <c r="G21" s="5"/>
+      <c r="H21" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I21" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="J21" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="K21" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L20" s="6" t="s">
+      <c r="L21" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="M21" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="N20" s="6" t="s">
+      <c r="N21" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="O20" s="6" t="s">
+      <c r="O21" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="P20" s="6" t="s">
+      <c r="P21" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="Q20" s="6" t="s">
+      <c r="Q21" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.3" footer="0.3"/>

</xml_diff>